<commit_message>
El programa es compatible con SQL Server y ademas ya se realizan inserciones ajax de las categorias y etiquetas, Se actualizo la carga de los datatables ya que primero se imprimian los datos y despues se les daba formato. Ahora los recibe directamente cada objeto de los datatables. Se iniciaron los filtros avanzados pero los quieren de otra forma asi que se inicia una reestructuracion, aun rehacer la creacion de la cadena unica ya que desean que el orden de los marcadores no importe.
</commit_message>
<xml_diff>
--- a/public/formatos/Importación_perfiles_formato.xlsx
+++ b/public/formatos/Importación_perfiles_formato.xlsx
@@ -109,9 +109,6 @@
     <t>Fecha de hallazgo</t>
   </si>
   <si>
-    <t>Fecha de desaparición</t>
-  </si>
-  <si>
     <t>Lugar de desaparición</t>
   </si>
   <si>
@@ -275,17 +272,27 @@
   </si>
   <si>
     <t>CURP del desaparecido</t>
+  </si>
+  <si>
+    <t>Fecha desaparición</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -421,59 +428,62 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="22" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="22" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -752,7 +762,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -762,7 +772,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CX76"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="BS1" workbookViewId="0">
+      <selection activeCell="BX1" sqref="BX1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -931,184 +943,184 @@
         <v>25</v>
       </c>
       <c r="AB1" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AC1" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD1" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE1" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="AD1" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE1" s="16" t="s">
+      <c r="AF1" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG1" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="AF1" s="16" t="s">
+      <c r="AH1" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI1" s="16" t="s">
         <v>62</v>
-      </c>
-      <c r="AG1" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="AH1" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AI1" s="16" t="s">
-        <v>63</v>
       </c>
       <c r="AJ1" s="16" t="s">
         <v>28</v>
       </c>
       <c r="AK1" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="AL1" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="AL1" s="16" t="s">
+      <c r="AM1" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="AM1" s="16" t="s">
+      <c r="AN1" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="AN1" s="16" t="s">
+      <c r="AO1" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="AO1" s="16" t="s">
+      <c r="AP1" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="AP1" s="16" t="s">
+      <c r="AQ1" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="AQ1" s="16" t="s">
+      <c r="AR1" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS1" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="AR1" s="16" t="s">
+      <c r="AT1" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="AU1" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV1" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="AW1" s="16" t="s">
         <v>60</v>
-      </c>
-      <c r="AS1" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="AT1" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="AU1" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="AV1" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="AW1" s="16" t="s">
-        <v>61</v>
       </c>
       <c r="AX1" s="16" t="s">
         <v>27</v>
       </c>
       <c r="AY1" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="AZ1" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="AZ1" s="16" t="s">
+      <c r="BA1" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="BA1" s="16" t="s">
+      <c r="BB1" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="BB1" s="16" t="s">
+      <c r="BC1" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="BC1" s="16" t="s">
-        <v>84</v>
-      </c>
       <c r="BD1" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="BE1" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="BE1" s="16" t="s">
+      <c r="BF1" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="BF1" s="16" t="s">
+      <c r="BG1" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="BG1" s="16" t="s">
+      <c r="BH1" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="BH1" s="16" t="s">
+      <c r="BI1" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="BI1" s="16" t="s">
+      <c r="BJ1" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="BJ1" s="16" t="s">
+      <c r="BK1" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="BK1" s="16" t="s">
+      <c r="BL1" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="BL1" s="16" t="s">
+      <c r="BM1" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="BM1" s="16" t="s">
+      <c r="BN1" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="BN1" s="16" t="s">
+      <c r="BO1" s="16" t="s">
         <v>74</v>
-      </c>
-      <c r="BO1" s="16" t="s">
-        <v>75</v>
       </c>
       <c r="BP1" s="8" t="s">
         <v>29</v>
       </c>
       <c r="BQ1" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BR1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="BS1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="BS1" s="8" t="s">
-        <v>39</v>
-      </c>
       <c r="BT1" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="BU1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="BV1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="BW1" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="BU1" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="BV1" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="BW1" s="9" t="s">
+      <c r="BX1" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="BY1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="BZ1" s="9" t="s">
         <v>78</v>
-      </c>
-      <c r="BX1" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="BY1" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="BZ1" s="9" t="s">
-        <v>79</v>
       </c>
       <c r="CA1" s="6" t="s">
         <v>30</v>
       </c>
       <c r="CB1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="CC1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="CC1" s="6" t="s">
+      <c r="CD1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="CD1" s="6" t="s">
-        <v>35</v>
-      </c>
       <c r="CE1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="CF1" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="CG1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="CF1" s="10" t="s">
+      <c r="CH1" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="CG1" s="7" t="s">
+      <c r="CI1" s="10" t="s">
         <v>42</v>
-      </c>
-      <c r="CH1" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="CI1" s="10" t="s">
-        <v>43</v>
       </c>
       <c r="CJ1" s="2"/>
       <c r="CK1" s="2"/>

</xml_diff>